<commit_message>
first commit latest by anjali
</commit_message>
<xml_diff>
--- a/DigitalCplusA/src/test/resources/TestData/TestData.xlsx
+++ b/DigitalCplusA/src/test/resources/TestData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15090" windowHeight="2265" firstSheet="12" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16110" windowHeight="4170" firstSheet="23" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
     <sheet name="Projectfiles" sheetId="2" r:id="rId2"/>
-    <sheet name="projecttimeline" sheetId="3" r:id="rId3"/>
-    <sheet name="communication" sheetId="4" r:id="rId4"/>
+    <sheet name="communication" sheetId="4" r:id="rId3"/>
+    <sheet name="projecttimeline" sheetId="29" r:id="rId4"/>
     <sheet name="communicationmeeting" sheetId="5" r:id="rId5"/>
     <sheet name="projectemail" sheetId="6" r:id="rId6"/>
     <sheet name="locatorrequest" sheetId="7" r:id="rId7"/>
@@ -24,13 +24,49 @@
     <sheet name="inventory" sheetId="15" r:id="rId15"/>
     <sheet name="supplieronly" sheetId="16" r:id="rId16"/>
     <sheet name="supplierinvoice" sheetId="17" r:id="rId17"/>
+    <sheet name="Budgetdashboard" sheetId="18" r:id="rId18"/>
+    <sheet name="Projectteam" sheetId="19" r:id="rId19"/>
+    <sheet name="Projectactivities" sheetId="20" r:id="rId20"/>
+    <sheet name="Sitevisit" sheetId="21" r:id="rId21"/>
+    <sheet name="Mytask" sheetId="22" r:id="rId22"/>
+    <sheet name="Actionitem" sheetId="23" r:id="rId23"/>
+    <sheet name="Asset" sheetId="24" r:id="rId24"/>
+    <sheet name="Announcement" sheetId="25" r:id="rId25"/>
+    <sheet name="punchlistmasters" sheetId="26" r:id="rId26"/>
+    <sheet name="techsupport" sheetId="27" r:id="rId27"/>
+    <sheet name="architecturalstagemaster" sheetId="28" r:id="rId28"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Author:
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="347">
   <si>
     <t>propertyadd</t>
   </si>
@@ -119,9 +155,6 @@
     <t>stage</t>
   </si>
   <si>
-    <t>processcheck</t>
-  </si>
-  <si>
     <t>startdate</t>
   </si>
   <si>
@@ -131,27 +164,9 @@
     <t>comments</t>
   </si>
   <si>
-    <t>updatecareof</t>
-  </si>
-  <si>
-    <t>PRE-DESIGN-PHASE</t>
-  </si>
-  <si>
-    <t>This is for Testing</t>
-  </si>
-  <si>
-    <t>Shayne Guzman</t>
-  </si>
-  <si>
-    <t>Zoning/Location Permits</t>
-  </si>
-  <si>
     <t>propertyname</t>
   </si>
   <si>
-    <t>computer</t>
-  </si>
-  <si>
     <t>project</t>
   </si>
   <si>
@@ -182,15 +197,9 @@
     <t>messagebody</t>
   </si>
   <si>
-    <t>Manny</t>
-  </si>
-  <si>
     <t>Testing</t>
   </si>
   <si>
-    <t>john</t>
-  </si>
-  <si>
     <t>11122020</t>
   </si>
   <si>
@@ -392,15 +401,9 @@
     <t>Architect</t>
   </si>
   <si>
-    <t>careof</t>
-  </si>
-  <si>
     <t>12112020</t>
   </si>
   <si>
-    <t>10112020</t>
-  </si>
-  <si>
     <t>selectstafftype</t>
   </si>
   <si>
@@ -768,13 +771,349 @@
   </si>
   <si>
     <t>Valerie Valdez</t>
+  </si>
+  <si>
+    <t>noofhours</t>
+  </si>
+  <si>
+    <t>edithrs1</t>
+  </si>
+  <si>
+    <t>SCHEMATIC DESIGN PHASE</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>type1</t>
+  </si>
+  <si>
+    <t>stafftype1</t>
+  </si>
+  <si>
+    <t>staff1</t>
+  </si>
+  <si>
+    <t>des</t>
+  </si>
+  <si>
+    <t>msg</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>chat1</t>
+  </si>
+  <si>
+    <t>Company Staff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Architect </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ann Dumaual </t>
+  </si>
+  <si>
+    <t>main staff</t>
+  </si>
+  <si>
+    <t>hey</t>
+  </si>
+  <si>
+    <t>hey,there</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valerie Valdez </t>
+  </si>
+  <si>
+    <t>stages</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>staffs</t>
+  </si>
+  <si>
+    <t>sdate</t>
+  </si>
+  <si>
+    <t>edate</t>
+  </si>
+  <si>
+    <t>eddate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRE-DESIGN PHASE </t>
+  </si>
+  <si>
+    <t>20122020</t>
+  </si>
+  <si>
+    <t>vdate</t>
+  </si>
+  <si>
+    <t>task</t>
+  </si>
+  <si>
+    <t>19122020</t>
+  </si>
+  <si>
+    <t>23122020</t>
+  </si>
+  <si>
+    <t>floor checking</t>
+  </si>
+  <si>
+    <t>check properly</t>
+  </si>
+  <si>
+    <t>25122020</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>priorities</t>
+  </si>
+  <si>
+    <t>assign</t>
+  </si>
+  <si>
+    <t>status1</t>
+  </si>
+  <si>
+    <t>estatus</t>
+  </si>
+  <si>
+    <t>slab checking</t>
+  </si>
+  <si>
+    <t>inspection</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>To Do</t>
+  </si>
+  <si>
+    <t>Doing</t>
+  </si>
+  <si>
+    <t>assets</t>
+  </si>
+  <si>
+    <t>floors</t>
+  </si>
+  <si>
+    <t>parentasset</t>
+  </si>
+  <si>
+    <t>modelnames</t>
+  </si>
+  <si>
+    <t>serialnos</t>
+  </si>
+  <si>
+    <t>purchasedates</t>
+  </si>
+  <si>
+    <t>vendorcontactnames</t>
+  </si>
+  <si>
+    <t>vendorphnos</t>
+  </si>
+  <si>
+    <t>vendoremails</t>
+  </si>
+  <si>
+    <t>warrantyfors</t>
+  </si>
+  <si>
+    <t>warrantytills</t>
+  </si>
+  <si>
+    <t>firstservicedues</t>
+  </si>
+  <si>
+    <t>nextservicedues</t>
+  </si>
+  <si>
+    <t>barcodes</t>
+  </si>
+  <si>
+    <t>assetscosts</t>
+  </si>
+  <si>
+    <t>depriciations</t>
+  </si>
+  <si>
+    <t>remindins</t>
+  </si>
+  <si>
+    <t>exisitingvendornames</t>
+  </si>
+  <si>
+    <t>vendor</t>
+  </si>
+  <si>
+    <t>Tv</t>
+  </si>
+  <si>
+    <t>Electrical</t>
+  </si>
+  <si>
+    <t>samsung</t>
+  </si>
+  <si>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>sam ele</t>
+  </si>
+  <si>
+    <t>8129981409</t>
+  </si>
+  <si>
+    <t>sam@gmail.com</t>
+  </si>
+  <si>
+    <t>12112021</t>
+  </si>
+  <si>
+    <t>12122020</t>
+  </si>
+  <si>
+    <t>12012021</t>
+  </si>
+  <si>
+    <t>11122</t>
+  </si>
+  <si>
+    <t>20000</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Months Before </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milan Paper Suppliers </t>
+  </si>
+  <si>
+    <t>new vendor</t>
+  </si>
+  <si>
+    <t>announcements</t>
+  </si>
+  <si>
+    <t>descriptions</t>
+  </si>
+  <si>
+    <t>dates</t>
+  </si>
+  <si>
+    <t>times</t>
+  </si>
+  <si>
+    <t>details</t>
+  </si>
+  <si>
+    <t>venus</t>
+  </si>
+  <si>
+    <t>Hoilday</t>
+  </si>
+  <si>
+    <t>holiday for all the staffs due to corona</t>
+  </si>
+  <si>
+    <t>25112020</t>
+  </si>
+  <si>
+    <t>1300</t>
+  </si>
+  <si>
+    <t>it will be paid leave</t>
+  </si>
+  <si>
+    <t>office</t>
+  </si>
+  <si>
+    <t>26112020</t>
+  </si>
+  <si>
+    <t>names</t>
+  </si>
+  <si>
+    <t>locations</t>
+  </si>
+  <si>
+    <t>reviewtypes</t>
+  </si>
+  <si>
+    <t>ename</t>
+  </si>
+  <si>
+    <t>manila</t>
+  </si>
+  <si>
+    <t>floor checking at manila</t>
+  </si>
+  <si>
+    <t>internal</t>
+  </si>
+  <si>
+    <t>floor tiles checking</t>
+  </si>
+  <si>
+    <t>issues</t>
+  </si>
+  <si>
+    <t>17112020</t>
+  </si>
+  <si>
+    <t>app is crashing</t>
+  </si>
+  <si>
+    <t>not working</t>
+  </si>
+  <si>
+    <t>design phase</t>
+  </si>
+  <si>
+    <t>selstage</t>
+  </si>
+  <si>
+    <t>procheck</t>
+  </si>
+  <si>
+    <t>seledate</t>
+  </si>
+  <si>
+    <t>ucareoff</t>
+  </si>
+  <si>
+    <t>21112020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Site Familiarization </t>
+  </si>
+  <si>
+    <t>John</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -787,6 +1126,25 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212529"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -814,11 +1172,13 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -826,6 +1186,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -872,7 +1240,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -904,9 +1272,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -938,6 +1307,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1113,14 +1483,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
@@ -1133,9 +1503,9 @@
     <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1168,9 +1538,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
-        <v>39</v>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>188</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -1213,70 +1583,70 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="F1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G1" t="s">
-        <v>110</v>
-      </c>
-      <c r="H1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1285,40 +1655,40 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="C1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>41</v>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>188</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1327,14 +1697,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
@@ -1351,68 +1721,68 @@
     <col min="18" max="18" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" t="s">
+        <v>122</v>
+      </c>
+      <c r="J1" t="s">
+        <v>123</v>
+      </c>
+      <c r="K1" t="s">
+        <v>124</v>
+      </c>
+      <c r="L1" t="s">
         <v>125</v>
       </c>
-      <c r="B1" t="s">
+      <c r="M1" t="s">
         <v>126</v>
       </c>
-      <c r="C1" t="s">
+      <c r="N1" t="s">
         <v>127</v>
       </c>
-      <c r="D1" t="s">
+      <c r="O1" t="s">
         <v>128</v>
       </c>
-      <c r="E1" t="s">
+      <c r="P1" t="s">
         <v>129</v>
       </c>
-      <c r="F1" t="s">
+      <c r="Q1" t="s">
         <v>130</v>
       </c>
-      <c r="G1" t="s">
+      <c r="R1" t="s">
         <v>131</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" t="s">
         <v>132</v>
-      </c>
-      <c r="I1" t="s">
-        <v>133</v>
-      </c>
-      <c r="J1" t="s">
-        <v>134</v>
-      </c>
-      <c r="K1" t="s">
-        <v>135</v>
-      </c>
-      <c r="L1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M1" t="s">
-        <v>137</v>
-      </c>
-      <c r="N1" t="s">
-        <v>138</v>
-      </c>
-      <c r="O1" t="s">
-        <v>139</v>
-      </c>
-      <c r="P1" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>141</v>
-      </c>
-      <c r="R1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18">
-      <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" t="s">
-        <v>143</v>
       </c>
       <c r="C2">
         <v>1234512345</v>
@@ -1421,46 +1791,46 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="F2" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="G2" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="L2">
         <v>23</v>
       </c>
       <c r="M2" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="N2" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="O2">
         <v>1234512345</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1473,14 +1843,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -1489,62 +1859,62 @@
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B1" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="C1" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="D1" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="E1" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="F1" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="G1" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="H1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="I1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>41</v>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>188</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="C2" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="D2" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="G2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="I2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1557,79 +1927,79 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H1" t="s">
+        <v>158</v>
+      </c>
+      <c r="I1" t="s">
         <v>163</v>
       </c>
-      <c r="C1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E1" t="s">
-        <v>166</v>
-      </c>
-      <c r="F1" t="s">
-        <v>167</v>
-      </c>
-      <c r="G1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H1" t="s">
-        <v>169</v>
-      </c>
-      <c r="I1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>41</v>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>188</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>234</v>
       </c>
       <c r="C2" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="F2" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="G2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H2" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="I2" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1639,14 +2009,14 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
@@ -1663,110 +2033,110 @@
     <col min="17" max="17" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1" t="s">
+        <v>169</v>
+      </c>
+      <c r="H1" t="s">
+        <v>181</v>
+      </c>
+      <c r="I1" t="s">
+        <v>170</v>
+      </c>
+      <c r="J1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K1" t="s">
+        <v>172</v>
+      </c>
+      <c r="L1" t="s">
+        <v>174</v>
+      </c>
+      <c r="M1" t="s">
         <v>175</v>
       </c>
-      <c r="C1" t="s">
+      <c r="N1" t="s">
         <v>176</v>
       </c>
-      <c r="D1" t="s">
+      <c r="O1" t="s">
         <v>177</v>
       </c>
-      <c r="E1" t="s">
+      <c r="P1" t="s">
         <v>178</v>
       </c>
-      <c r="F1" t="s">
+      <c r="Q1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
         <v>179</v>
       </c>
-      <c r="G1" t="s">
+      <c r="D2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="H1" t="s">
-        <v>192</v>
-      </c>
-      <c r="I1" t="s">
-        <v>181</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H2" t="s">
+        <v>232</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="K1" t="s">
+      <c r="J2" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="L1" t="s">
-        <v>185</v>
-      </c>
-      <c r="M1" t="s">
-        <v>186</v>
-      </c>
-      <c r="N1" t="s">
-        <v>187</v>
-      </c>
-      <c r="O1" t="s">
-        <v>188</v>
-      </c>
-      <c r="P1" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D2" t="s">
-        <v>244</v>
-      </c>
-      <c r="E2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H2" t="s">
-        <v>243</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="K2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="L2">
         <v>5000</v>
       </c>
       <c r="M2" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="N2" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="O2" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="P2" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="Q2" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -1776,14 +2146,14 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -1804,128 +2174,128 @@
     <col min="20" max="20" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B1" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="C1" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="D1" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="E1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" t="s">
+        <v>190</v>
+      </c>
+      <c r="H1" t="s">
+        <v>191</v>
+      </c>
+      <c r="I1" t="s">
+        <v>173</v>
+      </c>
+      <c r="J1" t="s">
+        <v>192</v>
+      </c>
+      <c r="K1" t="s">
+        <v>193</v>
+      </c>
+      <c r="L1" t="s">
+        <v>194</v>
+      </c>
+      <c r="M1" t="s">
+        <v>195</v>
+      </c>
+      <c r="N1" t="s">
+        <v>196</v>
+      </c>
+      <c r="O1" t="s">
+        <v>197</v>
+      </c>
+      <c r="P1" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>199</v>
+      </c>
+      <c r="R1" t="s">
         <v>200</v>
       </c>
-      <c r="F1" t="s">
-        <v>130</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="S1" t="s">
         <v>201</v>
       </c>
-      <c r="H1" t="s">
+      <c r="T1" t="s">
         <v>202</v>
       </c>
-      <c r="I1" t="s">
-        <v>184</v>
-      </c>
-      <c r="J1" t="s">
-        <v>203</v>
-      </c>
-      <c r="K1" t="s">
-        <v>204</v>
-      </c>
-      <c r="L1" t="s">
-        <v>205</v>
-      </c>
-      <c r="M1" t="s">
-        <v>206</v>
-      </c>
-      <c r="N1" t="s">
-        <v>207</v>
-      </c>
-      <c r="O1" t="s">
-        <v>208</v>
-      </c>
-      <c r="P1" t="s">
-        <v>209</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>210</v>
-      </c>
-      <c r="R1" t="s">
-        <v>211</v>
-      </c>
-      <c r="S1" t="s">
-        <v>212</v>
-      </c>
-      <c r="T1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="B2" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="E2" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="F2" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="G2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="H2" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="I2" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="J2" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="L2" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="M2" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="O2" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="P2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="S2" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="T2" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1938,14 +2308,14 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView topLeftCell="O1" workbookViewId="0">
       <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
@@ -1957,86 +2327,86 @@
     <col min="25" max="25" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B1" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="C1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G1" t="s">
+        <v>215</v>
+      </c>
+      <c r="H1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I1" t="s">
+        <v>216</v>
+      </c>
+      <c r="J1" t="s">
+        <v>172</v>
+      </c>
+      <c r="K1" t="s">
+        <v>217</v>
+      </c>
+      <c r="L1" t="s">
+        <v>218</v>
+      </c>
+      <c r="M1" t="s">
+        <v>219</v>
+      </c>
+      <c r="N1" t="s">
+        <v>220</v>
+      </c>
+      <c r="O1" t="s">
+        <v>119</v>
+      </c>
+      <c r="P1" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R1" t="s">
         <v>222</v>
       </c>
-      <c r="D1" t="s">
+      <c r="S1" t="s">
         <v>223</v>
       </c>
-      <c r="E1" t="s">
+      <c r="T1" t="s">
+        <v>230</v>
+      </c>
+      <c r="U1" t="s">
         <v>224</v>
       </c>
-      <c r="F1" t="s">
+      <c r="V1" t="s">
+        <v>146</v>
+      </c>
+      <c r="W1" t="s">
         <v>225</v>
       </c>
-      <c r="G1" t="s">
+      <c r="X1" t="s">
         <v>226</v>
       </c>
-      <c r="H1" t="s">
-        <v>180</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="Y1" t="s">
         <v>227</v>
       </c>
-      <c r="J1" t="s">
-        <v>183</v>
-      </c>
-      <c r="K1" t="s">
-        <v>228</v>
-      </c>
-      <c r="L1" t="s">
-        <v>229</v>
-      </c>
-      <c r="M1" t="s">
-        <v>230</v>
-      </c>
-      <c r="N1" t="s">
-        <v>231</v>
-      </c>
-      <c r="O1" t="s">
-        <v>130</v>
-      </c>
-      <c r="P1" t="s">
-        <v>232</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>138</v>
-      </c>
-      <c r="R1" t="s">
-        <v>233</v>
-      </c>
-      <c r="S1" t="s">
-        <v>234</v>
-      </c>
-      <c r="T1" t="s">
-        <v>241</v>
-      </c>
-      <c r="U1" t="s">
-        <v>235</v>
-      </c>
-      <c r="V1" t="s">
-        <v>157</v>
-      </c>
-      <c r="W1" t="s">
-        <v>236</v>
-      </c>
-      <c r="X1" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25">
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="B2">
         <v>12122020</v>
@@ -2048,7 +2418,7 @@
         <v>12152020</v>
       </c>
       <c r="E2" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F2">
         <v>12</v>
@@ -2063,25 +2433,25 @@
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="K2" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="L2" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="M2">
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="O2" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="P2" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="Q2" t="s">
         <v>9</v>
@@ -2096,19 +2466,130 @@
         <v>12122020</v>
       </c>
       <c r="U2" t="s">
+        <v>227</v>
+      </c>
+      <c r="V2" t="s">
+        <v>83</v>
+      </c>
+      <c r="W2" t="s">
+        <v>105</v>
+      </c>
+      <c r="X2" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>238</v>
       </c>
-      <c r="V2" t="s">
-        <v>92</v>
-      </c>
-      <c r="W2" t="s">
-        <v>114</v>
-      </c>
-      <c r="X2" t="s">
-        <v>190</v>
-      </c>
-      <c r="Y2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F1" t="s">
         <v>245</v>
+      </c>
+      <c r="G1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -2117,12 +2598,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
@@ -2130,7 +2613,7 @@
     <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -2147,7 +2630,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -2170,87 +2653,592 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>254</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>255</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>256</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>257</v>
       </c>
       <c r="E1" t="s">
-        <v>120</v>
+        <v>258</v>
       </c>
       <c r="F1" t="s">
-        <v>32</v>
+        <v>243</v>
       </c>
       <c r="G1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>122</v>
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>249</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>121</v>
+        <v>44</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" t="s">
-        <v>35</v>
+        <v>61</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>238</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>36</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D2" t="s">
+        <v>267</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>243</v>
+      </c>
+      <c r="G1" t="s">
+        <v>272</v>
+      </c>
+      <c r="H1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D2" t="s">
+        <v>249</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" t="s">
+        <v>238</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C1" t="s">
+        <v>280</v>
+      </c>
+      <c r="D1" t="s">
+        <v>281</v>
+      </c>
+      <c r="E1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G1" t="s">
+        <v>284</v>
+      </c>
+      <c r="H1" t="s">
+        <v>285</v>
+      </c>
+      <c r="I1" t="s">
+        <v>286</v>
+      </c>
+      <c r="J1" t="s">
+        <v>287</v>
+      </c>
+      <c r="K1" t="s">
+        <v>288</v>
+      </c>
+      <c r="L1" t="s">
+        <v>289</v>
+      </c>
+      <c r="M1" t="s">
+        <v>290</v>
+      </c>
+      <c r="N1" t="s">
+        <v>291</v>
+      </c>
+      <c r="O1" t="s">
+        <v>292</v>
+      </c>
+      <c r="P1" t="s">
+        <v>293</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>294</v>
+      </c>
+      <c r="R1" t="s">
+        <v>295</v>
+      </c>
+      <c r="S1" t="s">
+        <v>296</v>
+      </c>
+      <c r="T1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E2" t="s">
+        <v>300</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H2" t="s">
+        <v>302</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="T2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E1" t="s">
+        <v>318</v>
+      </c>
+      <c r="F1" t="s">
+        <v>319</v>
+      </c>
+      <c r="G1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="E2" t="s">
+        <v>324</v>
+      </c>
+      <c r="F2" t="s">
+        <v>325</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C1" t="s">
+        <v>315</v>
+      </c>
+      <c r="D1" t="s">
+        <v>329</v>
+      </c>
+      <c r="E1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C2" t="s">
+        <v>332</v>
+      </c>
+      <c r="D2" t="s">
+        <v>333</v>
+      </c>
+      <c r="E2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -2266,68 +3254,68 @@
     <col min="21" max="21" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
         <v>20</v>
       </c>
       <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
         <v>46</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H2" t="s">
         <v>47</v>
       </c>
-      <c r="I1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I2" t="s">
-        <v>52</v>
+      <c r="I2" s="5" t="s">
+        <v>346</v>
       </c>
       <c r="J2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2336,15 +3324,78 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="4" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>343</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
@@ -2359,74 +3410,74 @@
     <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" t="s">
         <v>58</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C2" t="s">
         <v>59</v>
-      </c>
-      <c r="E1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J1" t="s">
-        <v>65</v>
-      </c>
-      <c r="K1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" t="s">
-        <v>68</v>
       </c>
       <c r="D2">
         <v>123</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="G2" t="s">
-        <v>52</v>
+        <v>346</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="I2" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="J2" t="s">
         <v>9</v>
       </c>
       <c r="K2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2435,46 +3486,46 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>41</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>188</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2487,14 +3538,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
@@ -2502,44 +3553,44 @@
     <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="E1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>41</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>188</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2549,84 +3600,85 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
     <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="J2" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="I1" t="s">
-        <v>90</v>
-      </c>
-      <c r="J1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2635,14 +3687,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:N2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -2654,50 +3706,50 @@
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="D1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="E1" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="F1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
         <v>103</v>
       </c>
-      <c r="G1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" t="s">
-        <v>112</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>113</v>
+        <v>182</v>
       </c>
       <c r="D2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="E2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commited the latest code
</commit_message>
<xml_diff>
--- a/DigitalCplusA/src/test/resources/TestData/TestData.xlsx
+++ b/DigitalCplusA/src/test/resources/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16110" windowHeight="4170" firstSheet="23" activeTab="25"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16110" windowHeight="4170" firstSheet="23" activeTab="27"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="348">
   <si>
     <t>propertyadd</t>
   </si>
@@ -1107,6 +1107,9 @@
   </si>
   <si>
     <t>John</t>
+  </si>
+  <si>
+    <t>selproject1</t>
   </si>
 </sst>
 </file>
@@ -1487,7 +1490,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2488,39 +2491,48 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>235</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>238</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>239</v>
       </c>
     </row>
@@ -2532,63 +2544,73 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B1" t="s">
         <v>240</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>241</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>242</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>243</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>244</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>245</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>99</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>251</v>
       </c>
     </row>
@@ -2655,57 +2677,67 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B1" t="s">
         <v>254</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>255</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>256</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>257</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>258</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>243</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>261</v>
       </c>
     </row>
@@ -2716,51 +2748,60 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B1" t="s">
         <v>254</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>255</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>256</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>262</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>243</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>261</v>
       </c>
     </row>
@@ -2771,45 +2812,54 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B1" t="s">
         <v>257</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>258</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>263</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>243</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>266</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>267</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>268</v>
       </c>
     </row>
@@ -2820,68 +2870,75 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B1" t="s">
         <v>269</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>263</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>270</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>271</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>38</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>243</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>272</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" t="s">
         <v>274</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>275</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>249</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>238</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>278</v>
       </c>
     </row>
@@ -2892,141 +2949,150 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B1" t="s">
         <v>279</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>255</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>280</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>281</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>282</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>283</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>284</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>285</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>286</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>287</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>288</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>289</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>290</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>291</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>292</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>293</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>294</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>295</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>296</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" t="s">
         <v>298</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>299</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>82</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>299</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>300</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>302</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>313</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="K2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3034,57 +3100,66 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B1" t="s">
         <v>314</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>315</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>316</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>317</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>318</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>319</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" t="s">
         <v>320</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>321</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>324</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>325</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>326</v>
       </c>
     </row>
@@ -3095,52 +3170,59 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B1" t="s">
         <v>327</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>328</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>315</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>329</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" t="s">
         <v>266</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>331</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>332</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>333</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>334</v>
       </c>
     </row>
@@ -3151,38 +3233,45 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B1" t="s">
         <v>316</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>335</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>337</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>338</v>
       </c>
     </row>
@@ -3193,31 +3282,38 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>339</v>
       </c>
     </row>
@@ -3326,58 +3422,65 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="4" width="21.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="5" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B1" t="s">
         <v>340</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>341</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>342</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>343</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>238</v>
       </c>
     </row>

</xml_diff>

<commit_message>
pushed correct exe file
</commit_message>
<xml_diff>
--- a/DigitalCplusA/src/test/resources/TestData/TestData.xlsx
+++ b/DigitalCplusA/src/test/resources/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" firstSheet="17" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="350">
   <si>
     <t>propertyadd</t>
   </si>
@@ -1113,6 +1113,9 @@
   </si>
   <si>
     <t>21122020</t>
+  </si>
+  <si>
+    <t>visited</t>
   </si>
 </sst>
 </file>
@@ -2759,8 +2762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2808,7 +2811,7 @@
         <v>44</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>238</v>
+        <v>349</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>261</v>
@@ -3433,7 +3436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
final update by anjali
</commit_message>
<xml_diff>
--- a/DigitalCplusA/src/test/resources/TestData/TestData.xlsx
+++ b/DigitalCplusA/src/test/resources/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" firstSheet="17" activeTab="20"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" firstSheet="21" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="352">
   <si>
     <t>propertyadd</t>
   </si>
@@ -1116,6 +1116,12 @@
   </si>
   <si>
     <t>visited</t>
+  </si>
+  <si>
+    <t>vname</t>
+  </si>
+  <si>
+    <t>sam</t>
   </si>
 </sst>
 </file>
@@ -2762,7 +2768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -2961,18 +2967,24 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="8" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" customWidth="1"/>
+    <col min="13" max="13" width="15" customWidth="1"/>
+    <col min="14" max="14" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>346</v>
       </c>
@@ -2998,46 +3010,49 @@
         <v>284</v>
       </c>
       <c r="I1" t="s">
+        <v>350</v>
+      </c>
+      <c r="J1" t="s">
         <v>285</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>286</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>287</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>288</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>289</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>290</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>291</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>292</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>293</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>294</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>295</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>296</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>188</v>
       </c>
@@ -3062,49 +3077,52 @@
       <c r="H2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="J2" t="s">
         <v>302</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="U2" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>313</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="L2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated logs under child
</commit_message>
<xml_diff>
--- a/DigitalCplusA/src/test/resources/TestData/TestData.xlsx
+++ b/DigitalCplusA/src/test/resources/TestData/TestData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F56B4F8-E914-48BE-920C-67EDE9952464}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15240" windowHeight="3060" firstSheet="13" activeTab="16"/>
+    <workbookView xWindow="4670" yWindow="2210" windowWidth="14400" windowHeight="7350" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -37,17 +38,16 @@
     <sheet name="architecturalstagemaster" sheetId="28" r:id="rId28"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:N8"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="354">
   <si>
     <t>propertyadd</t>
   </si>
@@ -387,9 +387,6 @@
     <t>Drawing Materials</t>
   </si>
   <si>
-    <t>Computer</t>
-  </si>
-  <si>
     <t>20</t>
   </si>
   <si>
@@ -1125,19 +1122,19 @@
     <t>Anjali</t>
   </si>
   <si>
-    <t>mobile</t>
-  </si>
-  <si>
     <t>vendor company</t>
   </si>
   <si>
     <t>inv11109006</t>
+  </si>
+  <si>
+    <t>mobile1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1291,6 +1288,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1326,6 +1340,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1501,27 +1532,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -1556,9 +1587,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -1593,7 +1624,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -1601,21 +1632,22 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -1641,30 +1673,30 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>104</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>84</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>43</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1673,37 +1705,37 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>64</v>
       </c>
       <c r="B1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" t="s">
         <v>112</v>
       </c>
-      <c r="C1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C2" t="s">
         <v>84</v>
@@ -1715,92 +1747,92 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" t="s">
         <v>114</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>115</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>116</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>117</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>118</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>119</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>120</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>121</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>122</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>123</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>124</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>125</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>126</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>127</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>128</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>129</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>130</v>
       </c>
-      <c r="R1" t="s">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B2" t="s">
-        <v>132</v>
       </c>
       <c r="C2">
         <v>1234512345</v>
@@ -1809,51 +1841,51 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G2" t="s">
         <v>84</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="L2">
         <v>23</v>
       </c>
       <c r="M2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O2">
         <v>1234512345</v>
       </c>
       <c r="P2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -1861,69 +1893,69 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" t="s">
         <v>142</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>143</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" t="s">
         <v>144</v>
       </c>
-      <c r="E1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>145</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>146</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>147</v>
       </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>149</v>
-      </c>
-      <c r="D2" t="s">
-        <v>150</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G2" t="s">
         <v>43</v>
@@ -1937,7 +1969,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -1945,67 +1977,67 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7265625" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" t="s">
         <v>152</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>153</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>154</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>155</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>156</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>157</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C2" t="s">
         <v>158</v>
       </c>
-      <c r="I1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B2" t="s">
-        <v>231</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="F2" t="s">
         <v>84</v>
@@ -2014,7 +2046,7 @@
         <v>43</v>
       </c>
       <c r="H2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I2" t="s">
         <v>83</v>
@@ -2027,113 +2059,113 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" t="s">
         <v>164</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>165</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>166</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>167</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>168</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>180</v>
+      </c>
+      <c r="I1" t="s">
         <v>169</v>
       </c>
-      <c r="H1" t="s">
-        <v>181</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>170</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>171</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>173</v>
+      </c>
+      <c r="M1" t="s">
+        <v>174</v>
+      </c>
+      <c r="N1" t="s">
+        <v>175</v>
+      </c>
+      <c r="O1" t="s">
+        <v>176</v>
+      </c>
+      <c r="P1" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q1" t="s">
         <v>172</v>
       </c>
-      <c r="L1" t="s">
-        <v>174</v>
-      </c>
-      <c r="M1" t="s">
-        <v>175</v>
-      </c>
-      <c r="N1" t="s">
-        <v>176</v>
-      </c>
-      <c r="O1" t="s">
-        <v>177</v>
-      </c>
-      <c r="P1" t="s">
-        <v>178</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s">
         <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E2" t="s">
         <v>43</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>183</v>
       </c>
       <c r="K2" t="s">
         <v>43</v>
@@ -2142,19 +2174,19 @@
         <v>5000</v>
       </c>
       <c r="M2" t="s">
+        <v>183</v>
+      </c>
+      <c r="N2" t="s">
+        <v>186</v>
+      </c>
+      <c r="O2" t="s">
         <v>184</v>
       </c>
-      <c r="N2" t="s">
-        <v>187</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>185</v>
       </c>
-      <c r="P2" t="s">
-        <v>186</v>
-      </c>
       <c r="Q2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -2164,153 +2196,153 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" t="s">
         <v>114</v>
       </c>
-      <c r="B1" t="s">
-        <v>115</v>
-      </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" t="s">
         <v>189</v>
       </c>
-      <c r="F1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>190</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J1" t="s">
         <v>191</v>
       </c>
-      <c r="I1" t="s">
-        <v>173</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>192</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>193</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>194</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>195</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>196</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>197</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>198</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>199</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>200</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>201</v>
       </c>
-      <c r="T1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G2" t="s">
         <v>59</v>
       </c>
       <c r="H2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I2" t="s">
+        <v>203</v>
+      </c>
+      <c r="J2" t="s">
         <v>204</v>
       </c>
-      <c r="J2" t="s">
-        <v>205</v>
-      </c>
       <c r="K2" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="L2" t="s">
+        <v>208</v>
+      </c>
+      <c r="M2" t="s">
+        <v>132</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="L2" t="s">
-        <v>209</v>
-      </c>
-      <c r="M2" t="s">
-        <v>133</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>208</v>
-      </c>
       <c r="O2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P2" t="s">
         <v>43</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="S2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="T2" t="s">
         <v>83</v>
@@ -2318,7 +2350,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -2326,148 +2358,148 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="19" max="19" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.5703125" customWidth="1"/>
-    <col min="21" max="21" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" customWidth="1"/>
+    <col min="19" max="19" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.54296875" customWidth="1"/>
+    <col min="21" max="21" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D1" t="s">
         <v>210</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>211</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>212</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>213</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>168</v>
+      </c>
+      <c r="I1" t="s">
         <v>214</v>
       </c>
-      <c r="H1" t="s">
-        <v>169</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>171</v>
+      </c>
+      <c r="K1" t="s">
         <v>215</v>
       </c>
-      <c r="J1" t="s">
-        <v>172</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>216</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>217</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>218</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
+        <v>118</v>
+      </c>
+      <c r="P1" t="s">
         <v>219</v>
       </c>
-      <c r="O1" t="s">
-        <v>119</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
+        <v>126</v>
+      </c>
+      <c r="R1" t="s">
         <v>220</v>
       </c>
-      <c r="Q1" t="s">
-        <v>127</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>221</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
+        <v>228</v>
+      </c>
+      <c r="U1" t="s">
         <v>222</v>
       </c>
-      <c r="T1" t="s">
-        <v>229</v>
-      </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
+        <v>145</v>
+      </c>
+      <c r="W1" t="s">
         <v>223</v>
       </c>
-      <c r="V1" t="s">
-        <v>146</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>224</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>225</v>
       </c>
-      <c r="Y1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E2" t="s">
         <v>83</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>349</v>
-      </c>
       <c r="I2" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J2" t="s">
+        <v>226</v>
+      </c>
+      <c r="K2" t="s">
         <v>227</v>
       </c>
-      <c r="K2" t="s">
-        <v>228</v>
-      </c>
       <c r="L2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M2">
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="O2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P2" t="s">
         <v>82</v>
@@ -2476,16 +2508,16 @@
         <v>9</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="U2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="V2" t="s">
         <v>83</v>
@@ -2494,10 +2526,10 @@
         <v>105</v>
       </c>
       <c r="X2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Y2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -2507,50 +2539,50 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B1" t="s">
         <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D1" t="s">
         <v>20</v>
       </c>
       <c r="E1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>233</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>234</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -2560,75 +2592,75 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C1" t="s">
         <v>237</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>238</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>239</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>240</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>241</v>
-      </c>
-      <c r="G1" t="s">
-        <v>242</v>
       </c>
       <c r="H1" t="s">
         <v>99</v>
       </c>
       <c r="I1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>250</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -2637,24 +2669,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B1" t="s">
         <v>18</v>
@@ -2672,7 +2704,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -2699,57 +2731,57 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C1" t="s">
         <v>251</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>252</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>253</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>254</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>239</v>
+      </c>
+      <c r="H1" t="s">
         <v>255</v>
       </c>
-      <c r="G1" t="s">
-        <v>240</v>
-      </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>257</v>
-      </c>
       <c r="C2" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>245</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>246</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>44</v>
@@ -2758,10 +2790,10 @@
         <v>61</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -2770,62 +2802,62 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C1" t="s">
         <v>251</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>252</v>
       </c>
-      <c r="D1" t="s">
-        <v>253</v>
-      </c>
       <c r="E1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>257</v>
-      </c>
       <c r="C2" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>245</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>246</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>44</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -2834,56 +2866,56 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1" t="s">
         <v>254</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F1" t="s">
         <v>255</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E1" t="s">
-        <v>240</v>
-      </c>
-      <c r="F1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" t="s">
         <v>262</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>263</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -2892,77 +2924,77 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.26953125" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" customWidth="1"/>
+    <col min="3" max="3" width="13.7265625" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D1" t="s">
         <v>266</v>
       </c>
-      <c r="C1" t="s">
-        <v>260</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>267</v>
-      </c>
-      <c r="E1" t="s">
-        <v>268</v>
       </c>
       <c r="F1" t="s">
         <v>38</v>
       </c>
       <c r="G1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H1" t="s">
+        <v>268</v>
+      </c>
+      <c r="I1" t="s">
         <v>269</v>
       </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>271</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" t="s">
+        <v>245</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" t="s">
+        <v>234</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="E2" t="s">
-        <v>246</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G2" t="s">
-        <v>235</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>274</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -2971,231 +3003,231 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="8" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="23.5703125" customWidth="1"/>
-    <col min="11" max="11" width="17.7109375" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" customWidth="1"/>
+    <col min="8" max="9" width="12.7265625" customWidth="1"/>
+    <col min="10" max="10" width="23.54296875" customWidth="1"/>
+    <col min="11" max="11" width="17.7265625" customWidth="1"/>
+    <col min="12" max="12" width="18.54296875" customWidth="1"/>
     <col min="13" max="13" width="15" customWidth="1"/>
-    <col min="14" max="14" width="24.28515625" customWidth="1"/>
+    <col min="14" max="14" width="24.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D1" t="s">
         <v>276</v>
       </c>
-      <c r="C1" t="s">
-        <v>252</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>277</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>278</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>279</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>280</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>344</v>
+      </c>
+      <c r="J1" t="s">
         <v>281</v>
       </c>
-      <c r="I1" t="s">
-        <v>345</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>282</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>283</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>284</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>285</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>286</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>287</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>288</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>289</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>290</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>291</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>292</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>293</v>
       </c>
-      <c r="V1" t="s">
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>295</v>
-      </c>
-      <c r="C2" t="s">
-        <v>296</v>
       </c>
       <c r="D2" t="s">
         <v>82</v>
       </c>
       <c r="E2" t="s">
+        <v>295</v>
+      </c>
+      <c r="F2" t="s">
         <v>296</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="J2" t="s">
         <v>298</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="K2" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="2" t="s">
         <v>300</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>301</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="U2" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="V2" t="s">
         <v>309</v>
-      </c>
-      <c r="V2" t="s">
-        <v>310</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-1700-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C1" t="s">
         <v>311</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>312</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>313</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>314</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>315</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" t="s">
         <v>316</v>
       </c>
-      <c r="H1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>317</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" t="s">
         <v>320</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>321</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -3204,61 +3236,61 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.81640625" customWidth="1"/>
+    <col min="2" max="2" width="32.7265625" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="31.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.26953125" customWidth="1"/>
+    <col min="6" max="6" width="31.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C1" t="s">
         <v>324</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>311</v>
+      </c>
+      <c r="E1" t="s">
         <v>325</v>
       </c>
-      <c r="D1" t="s">
-        <v>312</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>326</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C2" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B2" t="s">
-        <v>263</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>328</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>329</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>330</v>
-      </c>
-      <c r="F2" t="s">
-        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -3267,47 +3299,47 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.26953125" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" customWidth="1"/>
+    <col min="3" max="3" width="23.1796875" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C1" t="s">
+        <v>331</v>
+      </c>
+      <c r="D1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="D1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" t="s">
         <v>333</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>334</v>
-      </c>
-      <c r="D2" t="s">
-        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -3316,40 +3348,40 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" customWidth="1"/>
+    <col min="3" max="3" width="25.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B1" t="s">
         <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>234</v>
+        <v>311</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" t="s">
+        <v>233</v>
       </c>
       <c r="C2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -3359,33 +3391,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -3417,18 +3449,18 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s">
         <v>43</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>44</v>
@@ -3443,7 +3475,7 @@
         <v>47</v>
       </c>
       <c r="I2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J2" t="s">
         <v>46</v>
@@ -3456,67 +3488,67 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="5" width="21.140625" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" customWidth="1"/>
+    <col min="3" max="3" width="21.7265625" customWidth="1"/>
+    <col min="4" max="5" width="21.1796875" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" customWidth="1"/>
+    <col min="7" max="7" width="23.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C1" t="s">
         <v>337</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>338</v>
-      </c>
-      <c r="D1" t="s">
-        <v>339</v>
       </c>
       <c r="E1" t="s">
         <v>30</v>
       </c>
       <c r="F1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C2" t="s">
+        <v>346</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="C2" t="s">
-        <v>347</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -3526,29 +3558,29 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -3583,9 +3615,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s">
         <v>58</v>
@@ -3603,7 +3635,7 @@
         <v>61</v>
       </c>
       <c r="G2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>62</v>
@@ -3624,21 +3656,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -3652,9 +3684,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>67</v>
@@ -3668,7 +3700,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -3676,22 +3708,22 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -3711,9 +3743,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>66</v>
@@ -3738,24 +3770,24 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" customWidth="1"/>
+    <col min="7" max="7" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -3787,18 +3819,18 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s">
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>61</v>
@@ -3825,26 +3857,22 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -3867,7 +3895,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -3875,22 +3903,23 @@
         <v>103</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D2" t="s">
         <v>105</v>
       </c>
       <c r="E2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated project action and property page
</commit_message>
<xml_diff>
--- a/DigitalCplusA/src/test/resources/TestData/TestData.xlsx
+++ b/DigitalCplusA/src/test/resources/TestData/TestData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608D2B4C-54A8-4A42-AF0D-8B80E7C380F8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4665" yWindow="2205" windowWidth="14400" windowHeight="7350" firstSheet="12" activeTab="25"/>
+    <workbookView xWindow="4670" yWindow="2210" windowWidth="14400" windowHeight="7350" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -41,12 +42,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1133,7 +1134,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1287,6 +1288,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1322,6 +1340,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1497,27 +1532,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -1552,7 +1587,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>187</v>
       </c>
@@ -1589,7 +1624,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -1597,22 +1632,22 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -1638,7 +1673,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>187</v>
       </c>
@@ -1670,21 +1705,21 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -1695,7 +1730,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>187</v>
       </c>
@@ -1712,31 +1747,31 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -1792,7 +1827,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>187</v>
       </c>
@@ -1850,7 +1885,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -1858,23 +1893,23 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -1903,7 +1938,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>187</v>
       </c>
@@ -1934,7 +1969,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -1942,24 +1977,24 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7265625" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -1988,7 +2023,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>187</v>
       </c>
@@ -2024,31 +2059,31 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -2101,7 +2136,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>187</v>
       </c>
@@ -2161,35 +2196,35 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -2251,7 +2286,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>187</v>
       </c>
@@ -2315,7 +2350,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -2323,27 +2358,27 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="19" max="19" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.5703125" customWidth="1"/>
-    <col min="21" max="21" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" customWidth="1"/>
+    <col min="19" max="19" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.54296875" customWidth="1"/>
+    <col min="21" max="21" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -2420,7 +2455,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>187</v>
       </c>
@@ -2504,19 +2539,19 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>340</v>
       </c>
@@ -2533,7 +2568,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>187</v>
       </c>
@@ -2557,20 +2592,20 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>340</v>
       </c>
@@ -2599,7 +2634,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>187</v>
       </c>
@@ -2634,22 +2669,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>341</v>
       </c>
@@ -2669,9 +2705,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s">
         <v>26</v>
@@ -2696,20 +2732,20 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>340</v>
       </c>
@@ -2735,7 +2771,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>187</v>
       </c>
@@ -2767,19 +2803,19 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>340</v>
       </c>
@@ -2802,7 +2838,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>187</v>
       </c>
@@ -2831,19 +2867,19 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>340</v>
       </c>
@@ -2863,7 +2899,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>187</v>
       </c>
@@ -2889,22 +2925,22 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.26953125" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" customWidth="1"/>
+    <col min="3" max="3" width="13.7265625" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>340</v>
       </c>
@@ -2933,7 +2969,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>187</v>
       </c>
@@ -2968,25 +3004,25 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="8" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="23.5703125" customWidth="1"/>
-    <col min="11" max="11" width="17.7109375" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" customWidth="1"/>
+    <col min="8" max="9" width="12.7265625" customWidth="1"/>
+    <col min="10" max="10" width="23.54296875" customWidth="1"/>
+    <col min="11" max="11" width="17.7265625" customWidth="1"/>
+    <col min="12" max="12" width="18.54296875" customWidth="1"/>
     <col min="13" max="13" width="15" customWidth="1"/>
-    <col min="14" max="14" width="24.28515625" customWidth="1"/>
+    <col min="14" max="14" width="24.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>340</v>
       </c>
@@ -3054,7 +3090,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>187</v>
       </c>
@@ -3124,26 +3160,26 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-1700-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>340</v>
       </c>
@@ -3169,7 +3205,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>187</v>
       </c>
@@ -3201,24 +3237,24 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.81640625" customWidth="1"/>
+    <col min="2" max="2" width="32.7265625" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="31.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.26953125" customWidth="1"/>
+    <col min="6" max="6" width="31.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>340</v>
       </c>
@@ -3238,7 +3274,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>187</v>
       </c>
@@ -3264,22 +3300,22 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.26953125" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" customWidth="1"/>
+    <col min="3" max="3" width="23.1796875" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>340</v>
       </c>
@@ -3293,7 +3329,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>187</v>
       </c>
@@ -3313,21 +3349,21 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" customWidth="1"/>
+    <col min="3" max="3" width="25.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>340</v>
       </c>
@@ -3338,7 +3374,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>187</v>
       </c>
@@ -3356,33 +3392,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -3414,7 +3450,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>187</v>
       </c>
@@ -3453,24 +3489,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="5" width="21.140625" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" customWidth="1"/>
+    <col min="3" max="3" width="21.7265625" customWidth="1"/>
+    <col min="4" max="5" width="21.1796875" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" customWidth="1"/>
+    <col min="7" max="7" width="23.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>340</v>
       </c>
@@ -3493,7 +3529,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>187</v>
       </c>
@@ -3523,29 +3559,29 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -3580,7 +3616,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>187</v>
       </c>
@@ -3621,21 +3657,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -3649,7 +3685,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>187</v>
       </c>
@@ -3665,7 +3701,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -3673,22 +3709,22 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -3708,7 +3744,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>187</v>
       </c>
@@ -3735,24 +3771,24 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.1796875" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" customWidth="1"/>
+    <col min="7" max="7" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -3784,7 +3820,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>187</v>
       </c>
@@ -3822,22 +3858,22 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -3860,7 +3896,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>34</v>
       </c>

</xml_diff>